<commit_message>
update Zeitbudget und Zeitplan
</commit_message>
<xml_diff>
--- a/documents/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yara\Dropbox\Studium\Semester 5\FrontendDevelopment1\FRONT_Projekt\front-projekt\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8DA049-3F30-495D-92CB-8EFABA174561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6519EE-D284-4C61-BDE6-71EADDDC75B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitbudget" sheetId="4" r:id="rId1"/>
@@ -1076,7 +1076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1166,6 +1166,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1398,8 +1399,8 @@
   <dimension ref="A1:L75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
+      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1534,15 +1535,15 @@
       </c>
       <c r="H6" s="33">
         <f>SUM(H10:H67)</f>
-        <v>42</v>
+        <v>45.5</v>
       </c>
       <c r="I6" s="30">
         <f>SUM(I10:I67)</f>
-        <v>49.5</v>
+        <v>52.5</v>
       </c>
       <c r="J6" s="31">
         <f>SUM(J10:J67)</f>
-        <v>32.75</v>
+        <v>39.75</v>
       </c>
       <c r="K6" s="25"/>
       <c r="L6" s="25"/>
@@ -1570,15 +1571,15 @@
       </c>
       <c r="H7" s="33">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>78</v>
+        <v>74.5</v>
       </c>
       <c r="I7" s="30">
         <f t="shared" si="1"/>
-        <v>70.5</v>
+        <v>67.5</v>
       </c>
       <c r="J7" s="31">
         <f t="shared" si="1"/>
-        <v>87.25</v>
+        <v>80.25</v>
       </c>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
@@ -1638,13 +1639,13 @@
         <v>121</v>
       </c>
       <c r="H10" s="25">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I10" s="25">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J10" s="25">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K10" s="25"/>
       <c r="L10" s="25"/>
@@ -1830,13 +1831,13 @@
         <v>133</v>
       </c>
       <c r="H16" s="25">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="I16" s="25">
         <v>1</v>
       </c>
       <c r="J16" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K16" s="25"/>
       <c r="L16" s="25"/>
@@ -1862,13 +1863,13 @@
         <v>135</v>
       </c>
       <c r="H17" s="25">
-        <v>3.25</v>
+        <v>5.25</v>
       </c>
       <c r="I17" s="25">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="J17" s="25">
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="K17" s="25"/>
       <c r="L17" s="25"/>
@@ -1949,10 +1950,10 @@
         <v>1</v>
       </c>
       <c r="I20" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" s="25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="25"/>
       <c r="L20" s="25"/>
@@ -2230,7 +2231,7 @@
         <v>203</v>
       </c>
       <c r="H30" s="25">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="I30" s="25">
         <v>4.5</v>
@@ -2268,7 +2269,7 @@
         <v>4</v>
       </c>
       <c r="J31" s="25">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="K31" s="25"/>
       <c r="L31" s="25"/>
@@ -2332,7 +2333,7 @@
         <v>5</v>
       </c>
       <c r="J33" s="25">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="K33" s="25"/>
       <c r="L33" s="25"/>
@@ -2428,7 +2429,7 @@
         <v>0</v>
       </c>
       <c r="J36" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K36" s="25"/>
       <c r="L36" s="25"/>
@@ -3354,11 +3355,11 @@
   </sheetPr>
   <dimension ref="A1:FJ1001"/>
   <sheetViews>
-    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="BB5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="CI43" sqref="CI43"/>
+      <selection pane="bottomRight" activeCell="CK25" sqref="CK25:CS25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.85546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4053,61 +4054,61 @@
       <c r="AO15" s="44"/>
       <c r="AP15" s="44"/>
       <c r="AQ15" s="44"/>
-      <c r="AR15" s="42"/>
-      <c r="AS15" s="42"/>
-      <c r="AT15" s="42"/>
-      <c r="AU15" s="42"/>
-      <c r="AV15" s="42"/>
-      <c r="AW15" s="42"/>
-      <c r="AX15" s="42"/>
-      <c r="AY15" s="42"/>
-      <c r="AZ15" s="42"/>
-      <c r="BA15" s="42"/>
-      <c r="BB15" s="42"/>
-      <c r="BC15" s="42"/>
-      <c r="BD15" s="42"/>
-      <c r="BE15" s="42"/>
-      <c r="BF15" s="42"/>
-      <c r="BG15" s="42"/>
-      <c r="BH15" s="42"/>
-      <c r="BI15" s="42"/>
-      <c r="BJ15" s="42"/>
-      <c r="BK15" s="42"/>
-      <c r="BL15" s="42"/>
-      <c r="BM15" s="42"/>
-      <c r="BN15" s="42"/>
-      <c r="BO15" s="42"/>
-      <c r="BP15" s="42"/>
-      <c r="BQ15" s="42"/>
-      <c r="BR15" s="42"/>
-      <c r="BS15" s="42"/>
-      <c r="BT15" s="42"/>
-      <c r="BU15" s="42"/>
-      <c r="BV15" s="42"/>
-      <c r="BW15" s="42"/>
-      <c r="BX15" s="42"/>
-      <c r="BY15" s="42"/>
-      <c r="BZ15" s="42"/>
-      <c r="CA15" s="42"/>
-      <c r="CB15" s="42"/>
-      <c r="CC15" s="42"/>
-      <c r="CD15" s="42"/>
-      <c r="CE15" s="42"/>
-      <c r="CF15" s="42"/>
-      <c r="CG15" s="42"/>
-      <c r="CH15" s="42"/>
-      <c r="CI15" s="42"/>
-      <c r="CJ15" s="42"/>
-      <c r="CK15" s="42"/>
-      <c r="CL15" s="42"/>
-      <c r="CM15" s="42"/>
-      <c r="CN15" s="42"/>
-      <c r="CO15" s="42"/>
-      <c r="CP15" s="42"/>
-      <c r="CQ15" s="42"/>
-      <c r="CR15" s="42"/>
-      <c r="CS15" s="42"/>
-      <c r="CT15" s="42"/>
+      <c r="AR15" s="44"/>
+      <c r="AS15" s="44"/>
+      <c r="AT15" s="44"/>
+      <c r="AU15" s="44"/>
+      <c r="AV15" s="44"/>
+      <c r="AW15" s="44"/>
+      <c r="AX15" s="44"/>
+      <c r="AY15" s="44"/>
+      <c r="AZ15" s="44"/>
+      <c r="BA15" s="44"/>
+      <c r="BB15" s="44"/>
+      <c r="BC15" s="44"/>
+      <c r="BD15" s="44"/>
+      <c r="BE15" s="44"/>
+      <c r="BF15" s="44"/>
+      <c r="BG15" s="44"/>
+      <c r="BH15" s="44"/>
+      <c r="BI15" s="44"/>
+      <c r="BJ15" s="44"/>
+      <c r="BK15" s="44"/>
+      <c r="BL15" s="44"/>
+      <c r="BM15" s="44"/>
+      <c r="BN15" s="44"/>
+      <c r="BO15" s="44"/>
+      <c r="BP15" s="44"/>
+      <c r="BQ15" s="44"/>
+      <c r="BR15" s="44"/>
+      <c r="BS15" s="44"/>
+      <c r="BT15" s="44"/>
+      <c r="BU15" s="44"/>
+      <c r="BV15" s="44"/>
+      <c r="BW15" s="44"/>
+      <c r="BX15" s="44"/>
+      <c r="BY15" s="44"/>
+      <c r="BZ15" s="44"/>
+      <c r="CA15" s="44"/>
+      <c r="CB15" s="44"/>
+      <c r="CC15" s="44"/>
+      <c r="CD15" s="44"/>
+      <c r="CE15" s="44"/>
+      <c r="CF15" s="44"/>
+      <c r="CG15" s="44"/>
+      <c r="CH15" s="44"/>
+      <c r="CI15" s="44"/>
+      <c r="CJ15" s="44"/>
+      <c r="CK15" s="44"/>
+      <c r="CL15" s="44"/>
+      <c r="CM15" s="44"/>
+      <c r="CN15" s="44"/>
+      <c r="CO15" s="44"/>
+      <c r="CP15" s="44"/>
+      <c r="CQ15" s="44"/>
+      <c r="CR15" s="44"/>
+      <c r="CS15" s="44"/>
+      <c r="CT15" s="44"/>
       <c r="CU15" s="42"/>
       <c r="CV15" s="42"/>
       <c r="CW15" s="42"/>
@@ -4125,19 +4126,19 @@
       <c r="C18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="CL18" s="42"/>
-      <c r="CM18" s="42"/>
-      <c r="CN18" s="42"/>
-      <c r="CO18" s="42"/>
-      <c r="CP18" s="42"/>
-      <c r="CQ18" s="42"/>
-      <c r="CR18" s="42"/>
-      <c r="CS18" s="42"/>
-      <c r="CT18" s="42"/>
-      <c r="CU18" s="42"/>
-      <c r="CV18" s="42"/>
-      <c r="CW18" s="42"/>
-      <c r="CX18" s="42"/>
+      <c r="CL18" s="61"/>
+      <c r="CM18" s="61"/>
+      <c r="CN18" s="61"/>
+      <c r="CO18" s="61"/>
+      <c r="CP18" s="61"/>
+      <c r="CQ18" s="61"/>
+      <c r="CR18" s="61"/>
+      <c r="CS18" s="61"/>
+      <c r="CT18" s="61"/>
+      <c r="CU18" s="61"/>
+      <c r="CV18" s="61"/>
+      <c r="CW18" s="61"/>
+      <c r="CX18" s="61"/>
     </row>
     <row r="19" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
@@ -4275,6 +4276,15 @@
       <c r="CH25" s="44"/>
       <c r="CI25" s="44"/>
       <c r="CJ25" s="44"/>
+      <c r="CK25" s="44"/>
+      <c r="CL25" s="44"/>
+      <c r="CM25" s="44"/>
+      <c r="CN25" s="44"/>
+      <c r="CO25" s="44"/>
+      <c r="CP25" s="44"/>
+      <c r="CQ25" s="44"/>
+      <c r="CR25" s="44"/>
+      <c r="CS25" s="44"/>
     </row>
     <row r="26" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
@@ -4419,6 +4429,15 @@
       <c r="CH29" s="44"/>
       <c r="CI29" s="44"/>
       <c r="CJ29" s="44"/>
+      <c r="CK29" s="44"/>
+      <c r="CL29" s="44"/>
+      <c r="CM29" s="44"/>
+      <c r="CN29" s="44"/>
+      <c r="CO29" s="44"/>
+      <c r="CP29" s="44"/>
+      <c r="CQ29" s="44"/>
+      <c r="CR29" s="44"/>
+      <c r="CS29" s="44"/>
     </row>
     <row r="30" spans="1:102" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
@@ -4631,6 +4650,15 @@
       <c r="CH33" s="44"/>
       <c r="CI33" s="44"/>
       <c r="CJ33" s="44"/>
+      <c r="CK33" s="44"/>
+      <c r="CL33" s="44"/>
+      <c r="CM33" s="44"/>
+      <c r="CN33" s="44"/>
+      <c r="CO33" s="44"/>
+      <c r="CP33" s="44"/>
+      <c r="CQ33" s="44"/>
+      <c r="CR33" s="44"/>
+      <c r="CS33" s="44"/>
     </row>
     <row r="34" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
@@ -4919,6 +4947,20 @@
       <c r="CH41" s="44"/>
       <c r="CI41" s="44"/>
       <c r="CJ41" s="39"/>
+      <c r="CK41" s="44"/>
+      <c r="CL41" s="44"/>
+      <c r="CM41" s="44"/>
+      <c r="CN41" s="44"/>
+      <c r="CO41" s="44"/>
+      <c r="CP41" s="44"/>
+      <c r="CQ41" s="44"/>
+      <c r="CR41" s="44"/>
+      <c r="CS41" s="44"/>
+      <c r="CT41" s="44"/>
+      <c r="CU41" s="44"/>
+      <c r="CV41" s="44"/>
+      <c r="CW41" s="44"/>
+      <c r="CX41" s="44"/>
     </row>
     <row r="42" spans="1:102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="36"/>
@@ -9238,13 +9280,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -9260,6 +9295,13 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
storage.js in index.html verlinken
</commit_message>
<xml_diff>
--- a/documents/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Besitzer\Dropbox\Studium\Semester 6\FRONT\FRONT_Projekt\front-projekt\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D782FDE8-6053-4D4F-B203-D88D699C1DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF507F4-A4E1-4874-BDBF-03A51D96D9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1421,8 +1421,8 @@
   <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I57" sqref="I57"/>
+      <pane ySplit="7" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="H6" s="31">
         <f>SUM(H10:H70)</f>
-        <v>53.75</v>
+        <v>54.25</v>
       </c>
       <c r="I6" s="28">
         <f>SUM(I10:I70)</f>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="H7" s="31">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>66.25</v>
+        <v>65.75</v>
       </c>
       <c r="I7" s="28">
         <f t="shared" si="1"/>
@@ -2901,7 +2901,7 @@
         <v>155</v>
       </c>
       <c r="H53" s="23">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I53" s="23"/>
       <c r="J53" s="23"/>
@@ -10220,13 +10220,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -10242,6 +10235,13 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
type bei id's von integer zu string ändern
</commit_message>
<xml_diff>
--- a/documents/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Besitzer\Dropbox\Studium\Semester 6\FRONT\FRONT_Projekt\front-projekt\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF507F4-A4E1-4874-BDBF-03A51D96D9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300B6C2F-9E02-4111-BD74-447AFCDAEA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1421,8 +1421,8 @@
   <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K63" sqref="K63"/>
+      <pane ySplit="7" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="H6" s="31">
         <f>SUM(H10:H70)</f>
-        <v>54.25</v>
+        <v>54.75</v>
       </c>
       <c r="I6" s="28">
         <f>SUM(I10:I70)</f>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="H7" s="31">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>65.75</v>
+        <v>65.25</v>
       </c>
       <c r="I7" s="28">
         <f t="shared" si="1"/>
@@ -1948,7 +1948,9 @@
       <c r="G19" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="H19" s="23"/>
+      <c r="H19" s="23">
+        <v>0.5</v>
+      </c>
       <c r="I19" s="23"/>
       <c r="J19" s="23">
         <v>0.5</v>
@@ -10220,6 +10222,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -10235,13 +10244,6 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Start und Ende von Leiterfeldern unterscheidbar machen
</commit_message>
<xml_diff>
--- a/documents/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Besitzer\Dropbox\Studium\Semester 6\FRONT\FRONT_Projekt\front-projekt\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300B6C2F-9E02-4111-BD74-447AFCDAEA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA48DF54-B5C7-437F-BF4B-819385FE2888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1421,8 +1421,8 @@
   <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
+      <pane ySplit="7" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="H6" s="31">
         <f>SUM(H10:H70)</f>
-        <v>54.75</v>
+        <v>55.25</v>
       </c>
       <c r="I6" s="28">
         <f>SUM(I10:I70)</f>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="H7" s="31">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>65.25</v>
+        <v>64.75</v>
       </c>
       <c r="I7" s="28">
         <f t="shared" si="1"/>
@@ -2596,7 +2596,9 @@
       <c r="G41" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="H41" s="23"/>
+      <c r="H41" s="23">
+        <v>0.5</v>
+      </c>
       <c r="I41" s="23"/>
       <c r="J41" s="23"/>
       <c r="K41" s="23"/>
@@ -10222,13 +10224,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -10244,6 +10239,13 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Kommentare für Einbinden der Serverkommunikation verfasst
</commit_message>
<xml_diff>
--- a/documents/Zeitbudget, -plan und Meilensteine.xlsx
+++ b/documents/Zeitbudget, -plan und Meilensteine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Besitzer\Dropbox\Studium\Semester 6\FRONT\FRONT_Projekt\front-projekt\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA48DF54-B5C7-437F-BF4B-819385FE2888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0096DF2-3F7C-49FC-A66B-45C11C243E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4605" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1421,8 +1421,8 @@
   <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I41" sqref="I41"/>
+      <pane ySplit="7" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1557,15 +1557,15 @@
       </c>
       <c r="H6" s="31">
         <f>SUM(H10:H70)</f>
-        <v>55.25</v>
+        <v>56.75</v>
       </c>
       <c r="I6" s="28">
         <f>SUM(I10:I70)</f>
-        <v>55</v>
+        <v>56.5</v>
       </c>
       <c r="J6" s="29">
         <f>SUM(J10:J70)</f>
-        <v>44.75</v>
+        <v>46.25</v>
       </c>
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
@@ -1593,15 +1593,15 @@
       </c>
       <c r="H7" s="31">
         <f t="shared" ref="H7:J7" si="1">H5-H6</f>
-        <v>64.75</v>
+        <v>63.25</v>
       </c>
       <c r="I7" s="28">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>63.5</v>
       </c>
       <c r="J7" s="29">
         <f t="shared" si="1"/>
-        <v>75.25</v>
+        <v>73.75</v>
       </c>
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
@@ -2905,10 +2905,14 @@
         <v>155</v>
       </c>
       <c r="H53" s="23">
+        <v>2</v>
+      </c>
+      <c r="I53" s="23">
         <v>1</v>
       </c>
-      <c r="I53" s="23"/>
-      <c r="J53" s="23"/>
+      <c r="J53" s="23">
+        <v>1</v>
+      </c>
       <c r="K53" s="23"/>
       <c r="L53" s="23"/>
     </row>
@@ -2993,10 +2997,14 @@
         <v>256</v>
       </c>
       <c r="H57" s="23">
-        <v>0.25</v>
-      </c>
-      <c r="I57" s="23"/>
-      <c r="J57" s="23"/>
+        <v>0.75</v>
+      </c>
+      <c r="I57" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="J57" s="23">
+        <v>0.5</v>
+      </c>
       <c r="K57" s="23"/>
       <c r="L57" s="23"/>
     </row>
@@ -10224,6 +10232,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AN1:AT1"/>
+    <mergeCell ref="AU1:BA1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="EH1:EN1"/>
     <mergeCell ref="EO1:EU1"/>
     <mergeCell ref="EV1:FB1"/>
@@ -10239,13 +10254,6 @@
     <mergeCell ref="DM1:DS1"/>
     <mergeCell ref="DT1:DZ1"/>
     <mergeCell ref="EA1:EG1"/>
-    <mergeCell ref="AN1:AT1"/>
-    <mergeCell ref="AU1:BA1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="AG1:AM1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>